<commit_message>
bergupdate: learned more on EaCoN and thought about what to do next: Should I really do slides right away?
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -404,9 +404,6 @@
     <t>fonctionne sur windows</t>
   </si>
   <si>
-    <t>ne fonctionne pas sur windows (bug connu des devs)</t>
-  </si>
-  <si>
     <t>image 1</t>
   </si>
   <si>
@@ -869,7 +866,12 @@
   <si>
     <t>Se base sur ASCAT, dont les spécificités sont:
 - prend en compte l'aneuploidie
-- prend en compte l'infiltration de cellules saines</t>
+- prend en compte l'infiltration de cellules saines
+Cela se traduit dans les résultats:
+- visualisation des éléments de LOH et copy number-neutral events</t>
+  </si>
+  <si>
+    <t>ne fonctionne pas sur windows (bug connu)</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1482,7 @@
     <col min="4" max="4" width="72.7109375" style="11" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="4"/>
     <col min="10" max="10" width="12" style="4" customWidth="1"/>
@@ -1506,13 +1508,13 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1542,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>7</v>
@@ -1557,7 +1559,7 @@
         <v>110</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1587,22 +1589,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>111</v>
+        <v>219</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1632,22 +1634,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>109</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1674,32 +1676,32 @@
     </row>
     <row r="5" spans="1:29" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>212</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -1730,13 +1732,13 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="3"/>
@@ -1745,13 +1747,13 @@
     </row>
     <row r="8" spans="1:29" s="8" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1782,13 +1784,13 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1863,7 +1865,7 @@
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -2910,7 +2912,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>26</v>
@@ -2960,7 +2962,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>38</v>
@@ -3114,7 +3116,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>60</v>
@@ -3340,19 +3342,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" t="s">
         <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>97</v>
@@ -3402,40 +3404,40 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" t="s">
         <v>126</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>127</v>
       </c>
-      <c r="D67" t="s">
-        <v>128</v>
-      </c>
       <c r="E67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C68">
         <v>6</v>
@@ -3444,18 +3446,18 @@
         <v>94609</v>
       </c>
       <c r="E68" t="s">
+        <v>130</v>
+      </c>
+      <c r="F68" t="s">
         <v>131</v>
       </c>
-      <c r="F68" t="s">
-        <v>132</v>
-      </c>
       <c r="G68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C69">
         <v>6</v>
@@ -3464,18 +3466,18 @@
         <v>110632</v>
       </c>
       <c r="E69" t="s">
+        <v>133</v>
+      </c>
+      <c r="F69" t="s">
         <v>134</v>
       </c>
-      <c r="F69" t="s">
-        <v>135</v>
-      </c>
       <c r="G69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70">
         <v>6</v>
@@ -3484,18 +3486,18 @@
         <v>133969</v>
       </c>
       <c r="E70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" t="s">
         <v>137</v>
       </c>
-      <c r="F70" t="s">
-        <v>138</v>
-      </c>
       <c r="G70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C71">
         <v>6</v>
@@ -3504,38 +3506,38 @@
         <v>151528</v>
       </c>
       <c r="E71" t="s">
+        <v>139</v>
+      </c>
+      <c r="F71" t="s">
         <v>140</v>
       </c>
-      <c r="F71" t="s">
-        <v>141</v>
-      </c>
       <c r="G71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" t="s">
         <v>150</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>151</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>152</v>
       </c>
-      <c r="D74" t="s">
-        <v>153</v>
-      </c>
       <c r="E74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3549,7 +3551,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C76">
         <v>19</v>
@@ -3563,33 +3565,33 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" t="s">
         <v>159</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>169</v>
+      </c>
+      <c r="E79" t="s">
+        <v>170</v>
+      </c>
+      <c r="F79" t="s">
+        <v>171</v>
+      </c>
+      <c r="G79" t="s">
         <v>160</v>
-      </c>
-      <c r="D79" t="s">
-        <v>170</v>
-      </c>
-      <c r="E79" t="s">
-        <v>171</v>
-      </c>
-      <c r="F79" t="s">
-        <v>172</v>
-      </c>
-      <c r="G79" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3604,12 +3606,12 @@
         <v>2632</v>
       </c>
       <c r="G80" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3624,12 +3626,12 @@
         <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3644,12 +3646,12 @@
         <v>2075</v>
       </c>
       <c r="G82" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3664,12 +3666,12 @@
         <v>4494</v>
       </c>
       <c r="G83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3684,12 +3686,12 @@
         <v>1950</v>
       </c>
       <c r="G84" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -3704,12 +3706,12 @@
         <v>2</v>
       </c>
       <c r="G85" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -3724,132 +3726,132 @@
         <v>5505</v>
       </c>
       <c r="G86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C89" t="s">
+        <v>178</v>
+      </c>
+      <c r="D89" t="s">
         <v>179</v>
-      </c>
-      <c r="D89" t="s">
-        <v>180</v>
       </c>
       <c r="E89" t="s">
         <v>107</v>
       </c>
       <c r="F89" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B90" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" t="s">
         <v>181</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>182</v>
       </c>
-      <c r="D90" t="s">
-        <v>183</v>
-      </c>
       <c r="E90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" t="s">
         <v>184</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>185</v>
       </c>
-      <c r="D91" t="s">
-        <v>186</v>
-      </c>
       <c r="E91" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" t="s">
         <v>187</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>188</v>
       </c>
-      <c r="D92" t="s">
-        <v>189</v>
-      </c>
       <c r="E92" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" t="s">
         <v>190</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>191</v>
       </c>
-      <c r="D93" t="s">
-        <v>192</v>
-      </c>
       <c r="E93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
+        <v>192</v>
+      </c>
+      <c r="C94" t="s">
         <v>193</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>194</v>
       </c>
-      <c r="D94" t="s">
-        <v>195</v>
-      </c>
       <c r="E94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" t="s">
         <v>196</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>197</v>
       </c>
-      <c r="D95" t="s">
-        <v>198</v>
-      </c>
       <c r="E95" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F95" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bergupdate: I read DNAcopy and took notes, reorganized a bit todo.md
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="221">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -637,22 +637,6 @@
     <t>PFB (population frequency of B alelle)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">PFB file. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CF. tableau 5</t>
-    </r>
-  </si>
-  <si>
     <t>input de genoCNA</t>
   </si>
   <si>
@@ -701,177 +685,170 @@
     <t>tableau 6</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The input column headers are:
+    <t>input de GISTIC</t>
+  </si>
+  <si>
+    <t>in cnchp files</t>
+  </si>
+  <si>
+    <t>in filename.segments.txt</t>
+  </si>
+  <si>
+    <t>( format:  CBS output)</t>
+  </si>
+  <si>
+    <t>File extension/type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>reference-file</t>
+  </si>
+  <si>
+    <t>REF_MODEL (HDF5)</t>
+  </si>
+  <si>
+    <t>Reference data generated by apt-copynumber-onco-ref</t>
+  </si>
+  <si>
+    <t>snp-qc-snp-list</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>SNP probes used in calculating SNP QC</t>
+  </si>
+  <si>
+    <t>annotation-file</t>
+  </si>
+  <si>
+    <t>annot.db (SQLite)</t>
+  </si>
+  <si>
+    <t>Annotation data for probes and probesets</t>
+  </si>
+  <si>
+    <t>x-probes-file</t>
+  </si>
+  <si>
+    <t>chrXprobes (text)</t>
+  </si>
+  <si>
+    <t>List of X-chromosome probes</t>
+  </si>
+  <si>
+    <t>y-probes-file</t>
+  </si>
+  <si>
+    <t>chrYprobes (text)</t>
+  </si>
+  <si>
+    <t>List of Y-chromosome probes</t>
+  </si>
+  <si>
+    <t>cel-pairs-file</t>
+  </si>
+  <si>
+    <t>tsv</t>
+  </si>
+  <si>
+    <t>Cel file pairs (AT and GC channel for each sample) for experiments</t>
+  </si>
+  <si>
+    <t>tableau 7</t>
+  </si>
+  <si>
+    <t>Actual name</t>
+  </si>
+  <si>
+    <t>OncoScan.FFPE.na33.r1.REF_MODEL</t>
+  </si>
+  <si>
+    <t>OncoScan.na33.r1.annot.db</t>
+  </si>
+  <si>
+    <t>OncoScan.r1.chrYprobes</t>
+  </si>
+  <si>
+    <t>OncoScan.r1.chrXprobes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OncoScan.r1.snplist.txt </t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>C:\Users\e.bordron\Desktop\CGH-scoring\library_files_oncoscan\OncoScan_Array_analysis_Files_NA33-r3</t>
+  </si>
+  <si>
+    <t>input of 
+apt-copynumber-onco-ssa</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fichier texte à 4 colonnes ayant pour lignes les sondes. Besoin du fichier CDF d'oncoscan -&gt; Tony Sierra
+OU
+d'utiliser apt-copynumber-onco-ssa -&gt; télécharger apt
+OU
+d'utiliser apt.oncoscan.2.4.0, une sous-partie d'EaCoN. -&gt; linux
+</t>
+  </si>
+  <si>
+    <t>valeurs LRR (CGHcall utilise les informations de breakpoint (par l'algo CBS, typiquement). Cela est envoyé vers un objet R: cghSeg
+https://www.rdocumentation.org/packages/CGHbase/versions/1.32.0/topics/cghSeg</t>
+  </si>
+  <si>
+    <t>classifie le LRR entre ref et tumeur en 5 états: double loss-homozygous (biallelic) deletion, loss-hemizygous deletion (loss of one of the alleles), normal-two copies, gain-three to four copies and amplification–more than four copies</t>
+  </si>
+  <si>
+    <t>résolution</t>
+  </si>
+  <si>
+    <t>calcul de différents scores de HRD</t>
+  </si>
+  <si>
+    <t>spécificité du package</t>
+  </si>
+  <si>
+    <t>système de visualisation interactive des données</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ne fonctionne pas sur windows (bug connu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - prend en compte la cellularité (on la renseigne)
+- un mixture model est utilisé (outil de clustering statistique) pour attribuer un état à chaque segment.</t>
+  </si>
+  <si>
+    <t>Se base sur ASCAT, dont les spécificités sont:
+- prend en compte l'aneuploidie
+- prend en compte la cellularité
+Cela se traduit dans les résultats:
+- visualisation des éléments de LOH et copy number-neutral events</t>
+  </si>
+  <si>
+    <t>DNAcopy</t>
+  </si>
+  <si>
+    <t>PFB file. CF. tableau 5</t>
+  </si>
+  <si>
+    <t>The input column headers are:
     (1)  Sample           (sample name)
     (2)  Chromosome  (chromosome number)
     (3)  Start Position  (segment start position, in bases)
     (4)  End Position   (segment end position, in bases)
     (5)  Num markers      (number of markers in segment)
     (6)  Seg.CN       (log2() -1 of copy number)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CF. tableau 6</t>
-    </r>
-  </si>
-  <si>
-    <t>input de GISTIC</t>
-  </si>
-  <si>
-    <t>in cnchp files</t>
-  </si>
-  <si>
-    <t>in filename.segments.txt</t>
-  </si>
-  <si>
-    <t>( format:  CBS output)</t>
-  </si>
-  <si>
-    <t>File extension/type</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>reference-file</t>
-  </si>
-  <si>
-    <t>REF_MODEL (HDF5)</t>
-  </si>
-  <si>
-    <t>Reference data generated by apt-copynumber-onco-ref</t>
-  </si>
-  <si>
-    <t>snp-qc-snp-list</t>
-  </si>
-  <si>
-    <t>txt</t>
-  </si>
-  <si>
-    <t>SNP probes used in calculating SNP QC</t>
-  </si>
-  <si>
-    <t>annotation-file</t>
-  </si>
-  <si>
-    <t>annot.db (SQLite)</t>
-  </si>
-  <si>
-    <t>Annotation data for probes and probesets</t>
-  </si>
-  <si>
-    <t>x-probes-file</t>
-  </si>
-  <si>
-    <t>chrXprobes (text)</t>
-  </si>
-  <si>
-    <t>List of X-chromosome probes</t>
-  </si>
-  <si>
-    <t>y-probes-file</t>
-  </si>
-  <si>
-    <t>chrYprobes (text)</t>
-  </si>
-  <si>
-    <t>List of Y-chromosome probes</t>
-  </si>
-  <si>
-    <t>cel-pairs-file</t>
-  </si>
-  <si>
-    <t>tsv</t>
-  </si>
-  <si>
-    <t>Cel file pairs (AT and GC channel for each sample) for experiments</t>
-  </si>
-  <si>
-    <t>tableau 7</t>
-  </si>
-  <si>
-    <t>Actual name</t>
-  </si>
-  <si>
-    <t>OncoScan.FFPE.na33.r1.REF_MODEL</t>
-  </si>
-  <si>
-    <t>OncoScan.na33.r1.annot.db</t>
-  </si>
-  <si>
-    <t>OncoScan.r1.chrYprobes</t>
-  </si>
-  <si>
-    <t>OncoScan.r1.chrXprobes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OncoScan.r1.snplist.txt </t>
-  </si>
-  <si>
-    <t>custom</t>
-  </si>
-  <si>
-    <t>C:\Users\e.bordron\Desktop\CGH-scoring\library_files_oncoscan\OncoScan_Array_analysis_Files_NA33-r3</t>
-  </si>
-  <si>
-    <t>input of 
-apt-copynumber-onco-ssa</t>
-  </si>
-  <si>
-    <t>CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fichier texte à 4 colonnes ayant pour lignes les sondes. Besoin du fichier CDF d'oncoscan -&gt; Tony Sierra
-OU
-d'utiliser apt-copynumber-onco-ssa -&gt; télécharger apt
-OU
-d'utiliser apt.oncoscan.2.4.0, une sous-partie d'EaCoN. -&gt; linux
-</t>
-  </si>
-  <si>
-    <t>valeurs LRR (CGHcall utilise les informations de breakpoint (par l'algo CBS, typiquement). Cela est envoyé vers un objet R: cghSeg
-https://www.rdocumentation.org/packages/CGHbase/versions/1.32.0/topics/cghSeg</t>
-  </si>
-  <si>
-    <t>classifie le LRR entre ref et tumeur en 5 états: double loss-homozygous (biallelic) deletion, loss-hemizygous deletion (loss of one of the alleles), normal-two copies, gain-three to four copies and amplification–more than four copies</t>
-  </si>
-  <si>
-    <t>résolution</t>
-  </si>
-  <si>
-    <t>calcul de différents scores de HRD</t>
-  </si>
-  <si>
-    <t>spécificité du package</t>
-  </si>
-  <si>
-    <t>système de visualisation interactive des données</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - prend en compte la cellularité (on la renseigne)
-- un mixture model est utilisé (outil de clustering statistique) pour mieux </t>
-  </si>
-  <si>
-    <t>Se base sur ASCAT, dont les spécificités sont:
-- prend en compte l'aneuploidie
-- prend en compte l'infiltration de cellules saines
-Cela se traduit dans les résultats:
-- visualisation des éléments de LOH et copy number-neutral events</t>
-  </si>
-  <si>
-    <t>ne fonctionne pas sur windows (bug connu)</t>
+CF. tableau 6</t>
   </si>
 </sst>
 </file>
@@ -1470,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,13 +1485,13 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1559,7 +1536,7 @@
         <v>110</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1601,10 +1578,10 @@
         <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1637,7 +1614,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>123</v>
@@ -1649,7 +1626,7 @@
         <v>115</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1679,18 +1656,18 @@
         <v>120</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>210</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1698,7 +1675,7 @@
         <v>117</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>148</v>
@@ -1732,28 +1709,24 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>218</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:29" s="8" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1782,28 +1755,35 @@
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>206</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="9"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -1865,7 +1845,7 @@
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -2962,7 +2942,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>38</v>
@@ -3348,13 +3328,13 @@
         <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>97</v>
@@ -3534,7 +3514,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
         <v>153</v>
@@ -3565,33 +3545,33 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" t="s">
         <v>158</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>168</v>
+      </c>
+      <c r="E79" t="s">
+        <v>169</v>
+      </c>
+      <c r="F79" t="s">
+        <v>170</v>
+      </c>
+      <c r="G79" t="s">
         <v>159</v>
-      </c>
-      <c r="D79" t="s">
-        <v>169</v>
-      </c>
-      <c r="E79" t="s">
-        <v>170</v>
-      </c>
-      <c r="F79" t="s">
-        <v>171</v>
-      </c>
-      <c r="G79" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3606,12 +3586,12 @@
         <v>2632</v>
       </c>
       <c r="G80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3626,12 +3606,12 @@
         <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3646,12 +3626,12 @@
         <v>2075</v>
       </c>
       <c r="G82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3666,12 +3646,12 @@
         <v>4494</v>
       </c>
       <c r="G83" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3686,12 +3666,12 @@
         <v>1950</v>
       </c>
       <c r="G84" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -3706,12 +3686,12 @@
         <v>2</v>
       </c>
       <c r="G85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -3726,132 +3706,132 @@
         <v>5505</v>
       </c>
       <c r="G86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B89" t="s">
         <v>150</v>
       </c>
       <c r="C89" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D89" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E89" t="s">
         <v>107</v>
       </c>
       <c r="F89" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B90" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" t="s">
+        <v>179</v>
+      </c>
+      <c r="D90" t="s">
         <v>180</v>
       </c>
-      <c r="C90" t="s">
-        <v>181</v>
-      </c>
-      <c r="D90" t="s">
-        <v>182</v>
-      </c>
       <c r="E90" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" t="s">
+        <v>182</v>
+      </c>
+      <c r="D91" t="s">
         <v>183</v>
       </c>
-      <c r="C91" t="s">
-        <v>184</v>
-      </c>
-      <c r="D91" t="s">
-        <v>185</v>
-      </c>
       <c r="E91" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>184</v>
+      </c>
+      <c r="C92" t="s">
+        <v>185</v>
+      </c>
+      <c r="D92" t="s">
         <v>186</v>
       </c>
-      <c r="C92" t="s">
-        <v>187</v>
-      </c>
-      <c r="D92" t="s">
-        <v>188</v>
-      </c>
       <c r="E92" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" t="s">
+        <v>188</v>
+      </c>
+      <c r="D93" t="s">
         <v>189</v>
       </c>
-      <c r="C93" t="s">
-        <v>190</v>
-      </c>
-      <c r="D93" t="s">
-        <v>191</v>
-      </c>
       <c r="E93" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
+        <v>190</v>
+      </c>
+      <c r="C94" t="s">
+        <v>191</v>
+      </c>
+      <c r="D94" t="s">
         <v>192</v>
       </c>
-      <c r="C94" t="s">
-        <v>193</v>
-      </c>
-      <c r="D94" t="s">
-        <v>194</v>
-      </c>
       <c r="E94" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" t="s">
+        <v>194</v>
+      </c>
+      <c r="D95" t="s">
         <v>195</v>
       </c>
-      <c r="C95" t="s">
-        <v>196</v>
-      </c>
-      <c r="D95" t="s">
-        <v>197</v>
-      </c>
       <c r="E95" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F95" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bergupdate: noted down things to do.
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="annexe" sheetId="2" r:id="rId2"/>
+    <sheet name="pipeline_view" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="224">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -849,6 +850,18 @@
     (5)  Num markers      (number of markers in segment)
     (6)  Seg.CN       (log2() -1 of copy number)
 CF. tableau 6</t>
+  </si>
+  <si>
+    <t>normalisation</t>
+  </si>
+  <si>
+    <t>segmentation L2R &amp; BAF par ASCAT
+centralisation
+calling</t>
+  </si>
+  <si>
+    <t>Estimation de la ploidie et de la cellularité
+Estimation du nombre de copies</t>
   </si>
 </sst>
 </file>
@@ -933,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -987,6 +1000,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1447,8 +1463,8 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,7 +2824,7 @@
   </sheetPr>
   <dimension ref="A3:P95"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
@@ -3849,4 +3865,46 @@
     <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bergupdate: I have read mixture model article from picard & al; I also started reading rCGH article. they use a GMM too, but for normalization
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -14,7 +14,6 @@
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="annexe" sheetId="2" r:id="rId2"/>
-    <sheet name="pipeline_view" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="221">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -850,18 +849,6 @@
     (5)  Num markers      (number of markers in segment)
     (6)  Seg.CN       (log2() -1 of copy number)
 CF. tableau 6</t>
-  </si>
-  <si>
-    <t>normalisation</t>
-  </si>
-  <si>
-    <t>segmentation L2R &amp; BAF par ASCAT
-centralisation
-calling</t>
-  </si>
-  <si>
-    <t>Estimation de la ploidie et de la cellularité
-Estimation du nombre de copies</t>
   </si>
 </sst>
 </file>
@@ -946,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1000,9 +987,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1463,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,7 +2809,7 @@
   <dimension ref="A3:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3865,46 +3849,4 @@
     <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>223</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
bergupdate: produced plots with CGHcall.R
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -1447,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bergupdate: EaCoN can't be installed on linux since it depends on facets. started to work on ASCAT only. also completed a bit CGHcall slides
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -1448,12 +1448,12 @@
   <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.28515625" style="11" customWidth="1"/>
     <col min="3" max="3" width="60.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="72.7109375" style="11" customWidth="1"/>

</xml_diff>

<commit_message>
bergupdate: ASCAT slides are done, started looking up and launched rCGH, also tried the interactive visualization app
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="220">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -427,9 +427,6 @@
 Score Tdplus (Tandem Duplication plus):
 Ce score est défini par le nombre de régions exprimant un gain d'une ou 2 copies (tandem duplication) et dont la taille est comprise entre 1 et 10 Mb. Le score TDplus a été lié à l'occurrence de tumeurs CDK12-deficient. Le gène CDK12 est impliqué dans la régulation de l'ARN polymérase 2, dont le dysfonctionnement va souvent de pair avec l'apparition de cancers.
 autres scores: average copy number variation, number of whole-genome doubling events, total number of Mbp altered …</t>
-  </si>
-  <si>
-    <t>potentiellement cross-platform</t>
   </si>
   <si>
     <t>OncoSNP</t>
@@ -492,55 +489,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
-l'output de segmentation (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">CF. tableau 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) est de la forme d'un output DNAcopy.
-Ce fichier peut être converti en tableau dont les gènes sont les lignes (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CF. tableau 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>CF. tableau 4</t>
   </si>
   <si>
@@ -789,14 +737,6 @@
   </si>
   <si>
     <t>CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fichier texte à 4 colonnes ayant pour lignes les sondes. Besoin du fichier CDF d'oncoscan -&gt; Tony Sierra
-OU
-d'utiliser apt-copynumber-onco-ssa -&gt; télécharger apt
-OU
-d'utiliser apt.oncoscan.2.4.0, une sous-partie d'EaCoN. -&gt; linux
-</t>
   </si>
   <si>
     <t>valeurs LRR (CGHcall utilise les informations de breakpoint (par l'algo CBS, typiquement). Cela est envoyé vers un objet R: cghSeg
@@ -849,6 +789,12 @@
     (5)  Num markers      (number of markers in segment)
     (6)  Seg.CN       (log2() -1 of copy number)
 CF. tableau 6</t>
+  </si>
+  <si>
+    <t>Fichier Probeset.txt généré par ChAS</t>
+  </si>
+  <si>
+    <t>Données de segmentation en format CBS ( DNAcopy), ou dans un tableau par gène</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1394,7 @@
   <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,13 +1431,13 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1536,7 +1482,7 @@
         <v>110</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1572,16 +1518,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1611,22 +1557,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>109</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1653,32 +1599,32 @@
     </row>
     <row r="5" spans="1:29" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -1709,7 +1655,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="16"/>
@@ -1720,13 +1666,13 @@
     </row>
     <row r="8" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1757,13 +1703,13 @@
     </row>
     <row r="9" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
@@ -1772,13 +1718,13 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
@@ -1845,7 +1791,7 @@
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -2892,7 +2838,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>26</v>
@@ -2942,7 +2888,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>38</v>
@@ -3096,7 +3042,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>60</v>
@@ -3322,19 +3268,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
         <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>97</v>
@@ -3394,30 +3340,30 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" t="s">
         <v>125</v>
       </c>
-      <c r="C67" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67" t="s">
-        <v>127</v>
-      </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C68">
         <v>6</v>
@@ -3426,18 +3372,18 @@
         <v>94609</v>
       </c>
       <c r="E68" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C69">
         <v>6</v>
@@ -3446,18 +3392,18 @@
         <v>110632</v>
       </c>
       <c r="E69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F69" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G69" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C70">
         <v>6</v>
@@ -3466,18 +3412,18 @@
         <v>133969</v>
       </c>
       <c r="E70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C71">
         <v>6</v>
@@ -3486,38 +3432,38 @@
         <v>151528</v>
       </c>
       <c r="E71" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" t="s">
         <v>149</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
         <v>150</v>
       </c>
-      <c r="C74" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" t="s">
-        <v>152</v>
-      </c>
       <c r="E74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3531,7 +3477,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C76">
         <v>19</v>
@@ -3545,33 +3491,33 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B79" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" t="s">
+        <v>166</v>
+      </c>
+      <c r="E79" t="s">
+        <v>167</v>
+      </c>
+      <c r="F79" t="s">
+        <v>168</v>
+      </c>
+      <c r="G79" t="s">
         <v>157</v>
-      </c>
-      <c r="C79" t="s">
-        <v>158</v>
-      </c>
-      <c r="D79" t="s">
-        <v>168</v>
-      </c>
-      <c r="E79" t="s">
-        <v>169</v>
-      </c>
-      <c r="F79" t="s">
-        <v>170</v>
-      </c>
-      <c r="G79" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3586,12 +3532,12 @@
         <v>2632</v>
       </c>
       <c r="G80" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3606,12 +3552,12 @@
         <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3626,12 +3572,12 @@
         <v>2075</v>
       </c>
       <c r="G82" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3646,12 +3592,12 @@
         <v>4494</v>
       </c>
       <c r="G83" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3666,12 +3612,12 @@
         <v>1950</v>
       </c>
       <c r="G84" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -3686,12 +3632,12 @@
         <v>2</v>
       </c>
       <c r="G85" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -3706,132 +3652,132 @@
         <v>5505</v>
       </c>
       <c r="G86" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B89" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C89" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D89" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E89" t="s">
         <v>107</v>
       </c>
       <c r="F89" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B90" t="s">
+        <v>176</v>
+      </c>
+      <c r="C90" t="s">
+        <v>177</v>
+      </c>
+      <c r="D90" t="s">
         <v>178</v>
       </c>
-      <c r="C90" t="s">
-        <v>179</v>
-      </c>
-      <c r="D90" t="s">
-        <v>180</v>
-      </c>
       <c r="E90" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91" t="s">
+        <v>180</v>
+      </c>
+      <c r="D91" t="s">
         <v>181</v>
       </c>
-      <c r="C91" t="s">
-        <v>182</v>
-      </c>
-      <c r="D91" t="s">
-        <v>183</v>
-      </c>
       <c r="E91" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" t="s">
+        <v>183</v>
+      </c>
+      <c r="D92" t="s">
         <v>184</v>
       </c>
-      <c r="C92" t="s">
-        <v>185</v>
-      </c>
-      <c r="D92" t="s">
-        <v>186</v>
-      </c>
       <c r="E92" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>185</v>
+      </c>
+      <c r="C93" t="s">
+        <v>186</v>
+      </c>
+      <c r="D93" t="s">
         <v>187</v>
       </c>
-      <c r="C93" t="s">
-        <v>188</v>
-      </c>
-      <c r="D93" t="s">
-        <v>189</v>
-      </c>
       <c r="E93" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" t="s">
         <v>190</v>
       </c>
-      <c r="C94" t="s">
-        <v>191</v>
-      </c>
-      <c r="D94" t="s">
-        <v>192</v>
-      </c>
       <c r="E94" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" t="s">
+        <v>192</v>
+      </c>
+      <c r="D95" t="s">
         <v>193</v>
       </c>
-      <c r="C95" t="s">
-        <v>194</v>
-      </c>
-      <c r="D95" t="s">
-        <v>195</v>
-      </c>
       <c r="E95" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F95" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bergupdate: worked on oncoscanR
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -749,9 +749,6 @@
     <t>résolution</t>
   </si>
   <si>
-    <t>calcul de différents scores de HRD</t>
-  </si>
-  <si>
     <t>spécificité du package</t>
   </si>
   <si>
@@ -795,6 +792,11 @@
   </si>
   <si>
     <t>Données de segmentation en format CBS ( DNAcopy), ou dans un tableau par gène</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- calcul de différents scores de HRD
+- donne une définition des altérations de bras chromosomique: si 80%  le bras subit une altération sur 80% de sa longueur au total, il est déclaré comme altéré.</t>
   </si>
 </sst>
 </file>
@@ -830,7 +832,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,6 +854,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -934,11 +942,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1059,7 +1077,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B21:F23" totalsRowShown="0">
   <autoFilter ref="B21:F23"/>
   <tableColumns count="5">
-    <tableColumn id="8" name="variable name"/>
+    <tableColumn id="8" name="variable name" dataDxfId="0"/>
     <tableColumn id="1" name="ProbeName"/>
     <tableColumn id="2" name=" ChrNum"/>
     <tableColumn id="3" name=" ChrStart"/>
@@ -1119,7 +1137,7 @@
     <tableColumn id="2" name="File extension/type"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="where to find it"/>
-    <tableColumn id="5" name="Actual name" dataDxfId="0"/>
+    <tableColumn id="5" name="Actual name" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1393,8 +1411,8 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1455,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1481,8 +1499,8 @@
       <c r="F2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>208</v>
+      <c r="G2" s="7" t="s">
+        <v>219</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1524,10 +1542,10 @@
         <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1560,10 +1578,10 @@
         <v>120</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>109</v>
@@ -1572,7 +1590,7 @@
         <v>110</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1613,7 +1631,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1655,7 +1673,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="16"/>
@@ -1709,7 +1727,7 @@
         <v>204</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
@@ -1724,7 +1742,7 @@
         <v>204</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
@@ -1791,7 +1809,7 @@
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -2754,8 +2772,8 @@
   </sheetPr>
   <dimension ref="A3:P95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,7 +3268,7 @@
       <c r="A21" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="21" t="s">
         <v>108</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -3270,7 +3288,7 @@
       <c r="A22" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="20" t="s">
         <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -3288,7 +3306,7 @@
     </row>
     <row r="23" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" t="s">
+      <c r="B23" s="20" t="s">
         <v>106</v>
       </c>
       <c r="C23" s="2" t="s">

</xml_diff>

<commit_message>
bergupdate: worked on oncoscanR code and slides, also ASCAT code for running samples
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="223">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>arm-level</t>
-  </si>
-  <si>
-    <t>text exported file from ChAS, only</t>
   </si>
   <si>
     <t>CEL files, only</t>
@@ -417,16 +414,6 @@
   </si>
   <si>
     <t>Les scores Log R et BAF  sont utilisés pour  déterminer la  segmentation du  génome</t>
-  </si>
-  <si>
-    <t>Computation of arm-level alteration. 
-Score LST (Large-scale State Transition):
-un LST est un breakpoint (point de séparation entre 2 segments ayant des valeurs de CN différentes) dont les 2 segments font plus de 10 Mb. Ce score, qui correspond au nombre de LST, est un bon indicateur de l'état du gène BRCA1 (dont l'inactivation est souvent constatée dans le carcinome du sein). BRCA1 participe au pathway de recombination homologue (un procédé de réparation de l'ADN lors d'un double-strand break), et sa mutation accompagne souvent les cancers du sein ou des ovaires. Une Homologous Recombination Deficiency (HRD) peut être déterminée par la mutation de BRCA1.
-Score LOH (Loss of Heterozygosity):
-Ce score correspond au nombre de segments présentant une perte d'hétérozygotie sur plus de 15 Mb. La perte d'hétérozygotie est la disparition d'un allèle sur un des deux chromosomes, supprimant du génome l'une des 2 copies de ce gène. Un lien entre ce score et une déficience du gène BRCA a été mis en évidence par les auteurs de l'article, ce qui indique que ce score est un bon indicateur de HRD.
-Score Tdplus (Tandem Duplication plus):
-Ce score est défini par le nombre de régions exprimant un gain d'une ou 2 copies (tandem duplication) et dont la taille est comprise entre 1 et 10 Mb. Le score TDplus a été lié à l'occurrence de tumeurs CDK12-deficient. Le gène CDK12 est impliqué dans la régulation de l'ARN polymérase 2, dont le dysfonctionnement va souvent de pair avec l'apparition de cancers.
-autres scores: average copy number variation, number of whole-genome doubling events, total number of Mbp altered …</t>
   </si>
   <si>
     <t>OncoSNP</t>
@@ -561,9 +548,6 @@
     <t>input rCGH</t>
   </si>
   <si>
-    <t>CEL files</t>
-  </si>
-  <si>
     <t>tableau 5</t>
   </si>
   <si>
@@ -737,13 +721,6 @@
   </si>
   <si>
     <t>CN</t>
-  </si>
-  <si>
-    <t>valeurs LRR (CGHcall utilise les informations de breakpoint (par l'algo CBS, typiquement). Cela est envoyé vers un objet R: cghSeg
-https://www.rdocumentation.org/packages/CGHbase/versions/1.32.0/topics/cghSeg</t>
-  </si>
-  <si>
-    <t>classifie le LRR entre ref et tumeur en 5 états: double loss-homozygous (biallelic) deletion, loss-hemizygous deletion (loss of one of the alleles), normal-two copies, gain-three to four copies and amplification–more than four copies</t>
   </si>
   <si>
     <t>résolution</t>
@@ -796,7 +773,40 @@
   <si>
     <t xml:space="preserve">
 - calcul de différents scores de HRD
-- donne une définition des altérations de bras chromosomique: si 80%  le bras subit une altération sur 80% de sa longueur au total, il est déclaré comme altéré.</t>
+- donne une définition des altérations de bras chromosomique: si  le bras subit une altération sur 80% de sa longueur au total, il est déclaré comme altéré.</t>
+  </si>
+  <si>
+    <t>Détermination des altérations arm-level avec une définition applicable en single-sample
+Calcul de scores de HRD</t>
+  </si>
+  <si>
+    <t>Fichiers CEL ou OSCHP</t>
+  </si>
+  <si>
+    <t>Segmentation ASPCF
+Calling ASCAT: estime et prend en compte la cellularité et la ploïdie
+Calcul de métriques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Données de Calling par sonde
+Données de Segmentation par sonde et par segment
+</t>
+  </si>
+  <si>
+    <t>Sondes</t>
+  </si>
+  <si>
+    <t>Fichier Segments.txt généré par ChAS</t>
+  </si>
+  <si>
+    <t>Segmentation ASPCF
+Le Calling estime et prend en compte la cellularité et la ploïdie, ce qui permet de tenir compte des événements de Copy Number neutre.</t>
+  </si>
+  <si>
+    <t>Nettoyage des données
+Deux normalisations
+Segmentation DNAcopy
+Calling par modèle de mélange de gaussiennes</t>
   </si>
 </sst>
 </file>
@@ -950,14 +960,6 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -974,6 +976,14 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1077,7 +1087,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B21:F23" totalsRowShown="0">
   <autoFilter ref="B21:F23"/>
   <tableColumns count="5">
-    <tableColumn id="8" name="variable name" dataDxfId="0"/>
+    <tableColumn id="8" name="variable name" dataDxfId="1"/>
     <tableColumn id="1" name="ProbeName"/>
     <tableColumn id="2" name=" ChrNum"/>
     <tableColumn id="3" name=" ChrStart"/>
@@ -1137,7 +1147,7 @@
     <tableColumn id="2" name="File extension/type"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="where to find it"/>
-    <tableColumn id="5" name="Actual name" dataDxfId="1"/>
+    <tableColumn id="5" name="Actual name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1409,10 +1419,10 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC137"/>
+  <dimension ref="A1:AC136"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,13 +1459,13 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1480,27 +1490,27 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="2" spans="1:29" s="8" customFormat="1" ht="309.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:29" s="5" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="B2" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>219</v>
+      <c r="F2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1525,27 +1535,27 @@
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
     </row>
-    <row r="3" spans="1:29" s="5" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G3" s="9" t="s">
+    <row r="3" spans="1:29" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>213</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1570,184 +1580,202 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="1:29" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:29" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="8" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-    </row>
-    <row r="5" spans="1:29" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+    </row>
+    <row r="8" spans="1:29" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:29" s="5" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="E10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-    </row>
-    <row r="9" spans="1:29" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -1768,7 +1796,7 @@
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1776,7 +1804,7 @@
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="19"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1800,7 +1828,9 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>205</v>
+      </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1808,9 +1838,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="10" t="s">
-        <v>210</v>
-      </c>
+      <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -2750,14 +2778,6 @@
       <c r="D136" s="10"/>
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
-      <c r="B137" s="10"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2772,7 +2792,7 @@
   </sheetPr>
   <dimension ref="A3:P95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -2806,69 +2826,69 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>20</v>
-      </c>
-      <c r="P4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F5" s="1">
         <v>58858172</v>
@@ -2880,45 +2900,45 @@
         <v>16043</v>
       </c>
       <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>34</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>35</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>36</v>
-      </c>
-      <c r="P5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1">
         <v>58859117</v>
@@ -2927,46 +2947,46 @@
         <v>58866549</v>
       </c>
       <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" t="s">
         <v>41</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F7" s="1">
         <v>52559169</v>
@@ -2978,28 +2998,28 @@
         <v>86267</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
         <v>47</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>48</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>49</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
         <v>50</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3028,216 +3048,216 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>57</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>58</v>
       </c>
-      <c r="I11" t="s">
-        <v>59</v>
-      </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E12" s="1">
         <v>249116709</v>
       </c>
       <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>64</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>65</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>66</v>
-      </c>
-      <c r="J12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E13" s="1">
         <v>242497851</v>
       </c>
       <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>71</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>72</v>
       </c>
-      <c r="I13" t="s">
-        <v>73</v>
-      </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E14" s="1">
         <v>197683938</v>
       </c>
       <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
         <v>76</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s">
         <v>77</v>
       </c>
-      <c r="H14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14" t="s">
-        <v>78</v>
-      </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E15" s="1">
         <v>190921709</v>
       </c>
       <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
         <v>81</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" t="s">
         <v>82</v>
       </c>
-      <c r="H15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" t="s">
-        <v>83</v>
-      </c>
       <c r="J15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E16" s="1">
         <v>180579439</v>
       </c>
       <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
         <v>86</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" t="s">
         <v>87</v>
       </c>
-      <c r="H16" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" t="s">
-        <v>88</v>
-      </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E17" s="1">
         <v>170849100</v>
       </c>
       <c r="F17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
         <v>91</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" t="s">
         <v>92</v>
       </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
-      </c>
       <c r="J17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3266,60 +3286,60 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3348,40 +3368,40 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" t="s">
+        <v>122</v>
+      </c>
+      <c r="D67" t="s">
         <v>123</v>
       </c>
-      <c r="C67" t="s">
-        <v>124</v>
-      </c>
-      <c r="D67" t="s">
-        <v>125</v>
-      </c>
       <c r="E67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C68">
         <v>6</v>
@@ -3390,18 +3410,18 @@
         <v>94609</v>
       </c>
       <c r="E68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G68" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C69">
         <v>6</v>
@@ -3410,18 +3430,18 @@
         <v>110632</v>
       </c>
       <c r="E69" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F69" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G69" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C70">
         <v>6</v>
@@ -3430,18 +3450,18 @@
         <v>133969</v>
       </c>
       <c r="E70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G70" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C71">
         <v>6</v>
@@ -3450,38 +3470,38 @@
         <v>151528</v>
       </c>
       <c r="E71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G71" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" t="s">
         <v>147</v>
       </c>
-      <c r="B74" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>150</v>
-      </c>
-      <c r="E74" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3495,7 +3515,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C76">
         <v>19</v>
@@ -3509,33 +3529,33 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B79" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C79" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D79" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F79" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G79" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3550,12 +3570,12 @@
         <v>2632</v>
       </c>
       <c r="G80" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3570,12 +3590,12 @@
         <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3590,12 +3610,12 @@
         <v>2075</v>
       </c>
       <c r="G82" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3610,12 +3630,12 @@
         <v>4494</v>
       </c>
       <c r="G83" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3630,12 +3650,12 @@
         <v>1950</v>
       </c>
       <c r="G84" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -3650,12 +3670,12 @@
         <v>2</v>
       </c>
       <c r="G85" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -3670,132 +3690,132 @@
         <v>5505</v>
       </c>
       <c r="G86" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B89" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C89" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D89" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F89" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D90" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E90" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C91" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D91" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E91" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D92" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E92" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C93" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D93" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E93" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C94" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D94" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E94" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C95" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D95" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E95" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F95" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bergupdate: wrote a plan of the internship report in md. gotta transpose it in overleaf (on chrome, it doesn't preview in firefox.
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="206">
   <si>
     <t>input</t>
   </si>
@@ -690,6 +690,9 @@
     <t>Utiliser ChAS pour exporter l'input
 Peut être automatisé: recentrer les données dans ChAS
 Lancer l'outil</t>
+  </si>
+  <si>
+    <t>ascat</t>
   </si>
 </sst>
 </file>
@@ -1290,8 +1293,8 @@
   </sheetPr>
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1507,9 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>205</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>

</xml_diff>

<commit_message>
bergupate: gotta read matmet feedback from elodie
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1447,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,7 +3684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>